<commit_message>
x,r,cost, empty cells, and distance between real and bus location
</commit_message>
<xml_diff>
--- a/src/egon/data/datasets/egon_etrago_line/scenarios.xlsx
+++ b/src/egon/data/datasets/egon_etrago_line/scenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\powerd-data\src\egon\data\datasets\egon_etrago_line\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D77430B-18F6-4241-A80B-A6FEADE5D02D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA70116-DFD9-4EBA-8D01-F69361581AE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>s_nom</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>total x</t>
+  </si>
+  <si>
+    <t>parallel cables</t>
   </si>
 </sst>
 </file>
@@ -164,11 +167,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -453,13 +457,16 @@
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.08984375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
@@ -610,6 +617,10 @@
         <f>2.5*10^6</f>
         <v>2500000</v>
       </c>
+      <c r="H6" s="4">
+        <f>G6/C6</f>
+        <v>1396.6480446927374</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
@@ -648,6 +659,12 @@
       <c r="K8" t="s">
         <v>18</v>
       </c>
+      <c r="L8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M8" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -664,6 +681,14 @@
       </c>
       <c r="K9">
         <v>567.16481358552301</v>
+      </c>
+      <c r="L9">
+        <f>18/3</f>
+        <v>6</v>
+      </c>
+      <c r="M9" s="4">
+        <f>G6/J9*K9/L9</f>
+        <v>20863.387646566978</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">

</xml_diff>